<commit_message>
removing data file if exists
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>testnamet1AQ</t>
-  </si>
-  <si>
-    <t>testnameAS</t>
-  </si>
-  <si>
-    <t>testnameNxVTg</t>
-  </si>
-  <si>
-    <t>testnameYnig</t>
-  </si>
-  <si>
-    <t>testnames</t>
+    <t>testname</t>
+  </si>
+  <si>
+    <t>testname1HY S Zqo</t>
+  </si>
+  <si>
+    <t>testname 4</t>
+  </si>
+  <si>
+    <t>testnameez B0hP</t>
+  </si>
+  <si>
+    <t>testnameHI</t>
   </si>
 </sst>
 </file>

</xml_diff>